<commit_message>
added explanation of "?" symbol to data dictionary
</commit_message>
<xml_diff>
--- a/Data Details 2021.xlsx
+++ b/Data Details 2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\College Case Competition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\229461\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07A4E2C-C055-4815-BC6F-2849ECFD7C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4EA2D29-521B-409E-A8C8-1F72F1F8A00F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C766D78-6290-4D1E-8E47-531A33547677}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C766D78-6290-4D1E-8E47-531A33547677}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId1"/>
@@ -443,9 +443,6 @@
     <t>Customer's age at time of 2013 vehicle purchase, in 10 year increments</t>
   </si>
   <si>
-    <t xml:space="preserve">A subset of nationwide used-car purchases for 2013, with vehicle purchase information, customer demographics, and post-purchase experience. The subset should be considered representative of the US used car market. The response variable is a count of vehicles purchased by the same customer at the same dealer in the 5 following years, 2014-2018. In your data, it's labeled as "Subsequent Purchases." </t>
-  </si>
-  <si>
     <t>Indicator (0,1) of whether the customer traded-in a vehicle they owned during the 2013 vehicle purchase</t>
   </si>
   <si>
@@ -465,6 +462,9 @@
   </si>
   <si>
     <t>In today’s marketplace, customers expect and demand a personalized experience. Given historical industry sales, how can CarMax tailor its marketing and inventory strategies to draw in distinct segments of consumers?</t>
+  </si>
+  <si>
+    <t>A subset of nationwide used-car purchases for 2013, with vehicle purchase information, customer demographics, and post-purchase experience. The subset should be considered representative of the US used car market. The response variable is a count of vehicles purchased by the same customer at the same dealer in the 5 following years, 2014-2018. In your data, it's labeled as "Subsequent Purchases." In all columns, a '?' symbol indicates null or missing values.</t>
   </si>
 </sst>
 </file>
@@ -868,38 +868,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D34EC4F-AF37-4EA3-B5EB-B8CD21560E3E}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="96.44140625" style="1" customWidth="1"/>
-    <col min="3" max="10" width="9.109375" style="1"/>
+    <col min="1" max="1" width="43.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="96.42578125" style="1" customWidth="1"/>
+    <col min="3" max="10" width="9.140625" style="1"/>
     <col min="11" max="11" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -908,7 +910,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -917,10 +919,10 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
@@ -931,7 +933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -942,7 +944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -953,7 +955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -964,7 +966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -975,7 +977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -986,18 +988,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1008,7 +1010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1019,7 +1021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1030,7 +1032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1041,56 +1043,56 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>

</xml_diff>